<commit_message>
Solved problem in the execution of bug_1264, Screenshots added to allure report
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="credentials" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <t>new_email</t>
   </si>
   <si>
-    <t>email@</t>
+    <t>email@111.222.333.44444</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,8 +431,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" display="mailto:email@111.222.333.44444"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>